<commit_message>
Update CODIGO HTML INCRUSTACION.xlsx
</commit_message>
<xml_diff>
--- a/CODIGO HTML INCRUSTACION.xlsx
+++ b/CODIGO HTML INCRUSTACION.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATA INTELLIGENCE Dropbox\DI Monitoreo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATA INTELLIGENCE Dropbox\DI Monitoreo II\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{848D83AC-9481-40DE-84E7-D23669C8DFB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB619661-1980-4425-A7D4-F8E9BBF25791}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{0EA5090D-AE2A-4762-9B72-07082E9F9299}"/>
   </bookViews>
@@ -283,25 +283,6 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color rgb="FFFF0000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
         <sz val="9"/>
         <color theme="1"/>
         <name val="Calibri"/>
@@ -309,50 +290,6 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF002060"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -460,13 +397,32 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -531,6 +487,50 @@
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF002060"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -559,8 +559,8 @@
       <xdr:row>6</xdr:row>
       <xdr:rowOff>144779</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+      <mc:Choice Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="2" name="DATA">
@@ -583,7 +583,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -637,8 +637,8 @@
       <xdr:row>6</xdr:row>
       <xdr:rowOff>121921</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+      <mc:Choice Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="3" name="Producto">
@@ -661,7 +661,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -733,24 +733,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{664B642E-5919-4A80-A883-251B00800FC4}" name="Incrustación_HTML" displayName="Incrustación_HTML" ref="A8:M25" totalsRowShown="0" headerRowDxfId="3" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{664B642E-5919-4A80-A883-251B00800FC4}" name="Incrustación_HTML" displayName="Incrustación_HTML" ref="A8:M25" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="A8:M25" xr:uid="{3A408A3B-74F1-4E14-AA55-57016F1D39D5}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{6D4601EE-69FB-4D52-814E-DBE3A92FB270}" name="DATA" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{0D01B9DE-29EC-4907-8BBB-CD56F49F28B8}" name="Producto" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{B91DF8C9-FF3C-4740-8609-15B88B6225B2}" name="Plataforma" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{FE4F1C77-B406-41EF-9B20-1D5E134125B9}" name="Título" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{5458B3A4-84C5-4C49-8417-5C8BE104EB44}" name="height (px)" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{E1E05544-235F-4E55-9C56-6ADEDA302543}" name="width (px)" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{7A3D9659-DFD7-4618-AB87-147430D18F18}" name="LINK" dataDxfId="0"/>
-    <tableColumn id="8" xr3:uid="{B20A9C8E-8D3C-4A97-80D1-C8E8DA3CF5B2}" name="HTML-Insertar" dataDxfId="1">
+    <tableColumn id="1" xr3:uid="{6D4601EE-69FB-4D52-814E-DBE3A92FB270}" name="DATA" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{0D01B9DE-29EC-4907-8BBB-CD56F49F28B8}" name="Producto" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{B91DF8C9-FF3C-4740-8609-15B88B6225B2}" name="Plataforma" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{FE4F1C77-B406-41EF-9B20-1D5E134125B9}" name="Título" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{5458B3A4-84C5-4C49-8417-5C8BE104EB44}" name="height (px)" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{E1E05544-235F-4E55-9C56-6ADEDA302543}" name="width (px)" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{7A3D9659-DFD7-4618-AB87-147430D18F18}" name="LINK" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{B20A9C8E-8D3C-4A97-80D1-C8E8DA3CF5B2}" name="HTML-Insertar" dataDxfId="5">
       <calculatedColumnFormula>+CONCATENATE(I9,J9,E9,K9,F9,L9,G9,M9)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{BD3519A1-E378-48D7-8E01-E620A5A6822E}" name="a" dataDxfId="9"/>
-    <tableColumn id="10" xr3:uid="{4BE4F734-A1D6-4DD2-8290-D71D6D4B1DA7}" name="b" dataDxfId="8"/>
-    <tableColumn id="11" xr3:uid="{18D484F4-90B9-4151-9273-2D5841C9EB13}" name="c" dataDxfId="7"/>
-    <tableColumn id="12" xr3:uid="{E6898821-2E97-45AC-B77C-4ABFD0859E2D}" name="d" dataDxfId="6"/>
-    <tableColumn id="13" xr3:uid="{DFF14490-1025-46EC-9D62-05DCA8FF1620}" name="e" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{BD3519A1-E378-48D7-8E01-E620A5A6822E}" name="a" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{4BE4F734-A1D6-4DD2-8290-D71D6D4B1DA7}" name="b" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{18D484F4-90B9-4151-9273-2D5841C9EB13}" name="c" dataDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{E6898821-2E97-45AC-B77C-4ABFD0859E2D}" name="d" dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{DFF14490-1025-46EC-9D62-05DCA8FF1620}" name="e" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1057,7 +1057,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>